<commit_message>
analysis notebook, logging, refactoring
</commit_message>
<xml_diff>
--- a/duration_estimation.xlsx
+++ b/duration_estimation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\human_planning_horizon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9E7067-93B3-46BF-B9EE-FDD6E3B5C204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10E9DB5-69E2-42CB-8A54-2A6FB0321C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
   <dimension ref="A2:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,13 +512,13 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -542,11 +542,11 @@
       </c>
       <c r="C5" s="8">
         <f>$B$2 *B5</f>
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="D5" s="9">
         <f>C5/60</f>
-        <v>3.75</v>
+        <v>4.166666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -554,15 +554,15 @@
         <v>0</v>
       </c>
       <c r="B6" s="8">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C6" s="8">
         <f t="shared" ref="C6:C8" si="0">$B$2 *B6</f>
-        <v>900</v>
+        <v>750</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" ref="D6:D8" si="1">C6/60</f>
-        <v>15</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -570,15 +570,15 @@
         <v>1</v>
       </c>
       <c r="B7" s="8">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>750</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -586,15 +586,15 @@
         <v>2</v>
       </c>
       <c r="B8" s="5">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>750</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -603,15 +603,15 @@
       </c>
       <c r="B10" s="2">
         <f>SUM(B5:B8)</f>
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2">
         <f>SUM(C5:C8)</f>
-        <v>2925</v>
+        <v>2500</v>
       </c>
       <c r="D10" s="3">
         <f>C10/60</f>
-        <v>48.75</v>
+        <v>41.666666666666664</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -620,15 +620,15 @@
       </c>
       <c r="B11" s="5">
         <f>SUM(B5:B8)</f>
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C11" s="5">
         <f>SUM(B5:B8)*D2</f>
-        <v>3900</v>
+        <v>3750</v>
       </c>
       <c r="D11" s="6">
         <f>C11/60</f>
-        <v>65</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>